<commit_message>
Added and updated files.
</commit_message>
<xml_diff>
--- a/notebooks/Foreground.xlsx
+++ b/notebooks/Foreground.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreavargasf/ua_pmlca/ua_pmlca/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8847AB60-DD29-504D-9235-CA5097516D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF47100C-E885-DF44-97CE-C08B58F3A28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32880" yWindow="4480" windowWidth="27280" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32960" yWindow="5640" windowWidth="27280" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="J272" sqref="J272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -5673,10 +5673,6 @@
         <f t="shared" si="24"/>
         <v>(unknown)</v>
       </c>
-      <c r="I261" s="1">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
       <c r="J261" s="1">
         <f t="shared" si="24"/>
         <v>0</v>
@@ -5715,10 +5711,6 @@
         <f t="shared" si="26"/>
         <v>(unknown)</v>
       </c>
-      <c r="I262" s="1">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
       <c r="J262" s="1">
         <f t="shared" si="26"/>
         <v>0</v>
@@ -5757,10 +5749,6 @@
         <f t="shared" si="27"/>
         <v>(unknown)</v>
       </c>
-      <c r="I263" s="1">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
       <c r="J263" s="1">
         <f t="shared" si="27"/>
         <v>0</v>
@@ -5799,10 +5787,6 @@
         <f t="shared" si="28"/>
         <v>(unknown)</v>
       </c>
-      <c r="I264" s="1">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="J264" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
@@ -5841,10 +5825,6 @@
         <f t="shared" si="29"/>
         <v>(unknown)</v>
       </c>
-      <c r="I265" s="1">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
       <c r="J265" s="1">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -5883,10 +5863,6 @@
         <f t="shared" si="30"/>
         <v>(unknown)</v>
       </c>
-      <c r="I266" s="1">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
       <c r="J266" s="1">
         <f t="shared" si="30"/>
         <v>0</v>
@@ -5925,10 +5901,6 @@
         <f t="shared" si="31"/>
         <v>(unknown)</v>
       </c>
-      <c r="I267" s="1">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
       <c r="J267" s="1">
         <f t="shared" si="31"/>
         <v>0</v>
@@ -5967,10 +5939,6 @@
         <f t="shared" si="32"/>
         <v>(unknown)</v>
       </c>
-      <c r="I268" s="1">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
       <c r="J268" s="1">
         <f t="shared" si="32"/>
         <v>0</v>
@@ -6008,10 +5976,6 @@
       <c r="H269" s="1" t="str">
         <f t="shared" si="33"/>
         <v>(unknown)</v>
-      </c>
-      <c r="I269" s="1">
-        <f t="shared" si="33"/>
-        <v>0</v>
       </c>
       <c r="J269" s="1">
         <f t="shared" si="33"/>

</xml_diff>